<commit_message>
#23 delete and delete all buttons added
</commit_message>
<xml_diff>
--- a/test_files/file3.xlsx
+++ b/test_files/file3.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
   <si>
     <t xml:space="preserve">İsim</t>
   </si>
@@ -50,6 +50,12 @@
   </si>
   <si>
     <t xml:space="preserve">Mimar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yunus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Şen</t>
   </si>
   <si>
     <t xml:space="preserve">Mehmet</t>
@@ -68,7 +74,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -90,14 +96,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -154,7 +152,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -175,20 +173,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
+      <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.53"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.46"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="14.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="14.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1023" min="5" style="0" width="8.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1024" style="0" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -206,45 +199,59 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="0" t="s">
         <v>5</v>
       </c>
       <c r="C2" s="0" t="n">
-        <v>5055555555</v>
+        <v>5305555555</v>
       </c>
       <c r="D2" s="0" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B3" s="0" t="s">
         <v>8</v>
       </c>
       <c r="C3" s="0" t="n">
-        <v>5055555555</v>
+        <v>5305555555</v>
       </c>
       <c r="D3" s="0" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B4" s="0" t="s">
         <v>11</v>
       </c>
       <c r="C4" s="0" t="n">
+        <v>5305555555</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="0" t="n">
         <v>5055555555</v>
       </c>
-      <c r="D4" s="0" t="s">
-        <v>12</v>
+      <c r="D5" s="0" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>